<commit_message>
ajout de l'entete dans la revue de code
</commit_message>
<xml_diff>
--- a/TP1/revue_code/revue_code_Amar.xlsx
+++ b/TP1/revue_code/revue_code_Amar.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramah\Desktop\420-5GP-BB - TP1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramah\Desktop\truc au pif 2\cegep\21-AU\maintenance logiciel\TP1\TP1-420-5GP-BB\TP1\revue_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6339610F-DC60-4643-823C-F1A02D5272C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{701673DA-C7E0-4611-B04C-039DA74F0EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15285" yWindow="5565" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2685" yWindow="2160" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="46">
   <si>
     <t>FICHE DE RÉVISION DE CODE</t>
   </si>
@@ -142,6 +142,27 @@
   </si>
   <si>
     <t>14-45</t>
+  </si>
+  <si>
+    <t>GeoBomber.py</t>
+  </si>
+  <si>
+    <t>Éric Drouin</t>
+  </si>
+  <si>
+    <t>Amar Hadjeres</t>
+  </si>
+  <si>
+    <t>GeoBomber</t>
+  </si>
+  <si>
+    <t>03/10/2021</t>
+  </si>
+  <si>
+    <t>29/09/2021</t>
+  </si>
+  <si>
+    <t>17/10/2021</t>
   </si>
 </sst>
 </file>
@@ -215,14 +236,14 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -540,7 +561,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -555,78 +576,102 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>39</v>
+      </c>
       <c r="E3" t="s">
         <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>3</v>
       </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
       <c r="E4" t="s">
         <v>4</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>5</v>
       </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
       <c r="E5" t="s">
         <v>6</v>
+      </c>
+      <c r="F5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>7</v>
       </c>
+      <c r="F6" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>8</v>
       </c>
+      <c r="D7">
+        <v>50</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="G11" s="2" t="s">
         <v>17</v>
       </c>
     </row>
@@ -818,7 +863,7 @@
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D28" s="4"/>
+      <c r="D28" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>